<commit_message>
fixed big errors in fit
</commit_message>
<xml_diff>
--- a/exponent_calculation/Exponents.xlsx
+++ b/exponent_calculation/Exponents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3xpl0r3r\Documents\CP_sandpile\exponent_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C155C2-6D05-4F4D-BDCC-69F814868447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767317DB-8505-4E08-AD0C-5C2D5E9EEB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DFAB4312-AA51-4AEB-B081-BB1E149BA264}"/>
   </bookViews>
@@ -113,39 +113,9 @@
     <t>100</t>
   </si>
   <si>
-    <t>1.41+/-0.18</t>
-  </si>
-  <si>
-    <t>1.5+/-1.2</t>
-  </si>
-  <si>
-    <t>0.0336561226968521</t>
-  </si>
-  <si>
-    <t>0.0235441093811112</t>
-  </si>
-  <si>
-    <t>1.415383767004484</t>
-  </si>
-  <si>
     <t>E_of_S_T</t>
   </si>
   <si>
-    <t>0.50+/-0.21</t>
-  </si>
-  <si>
-    <t>1.6+/-0.5</t>
-  </si>
-  <si>
-    <t>0.0433618650058831</t>
-  </si>
-  <si>
-    <t>0.1039824912134339</t>
-  </si>
-  <si>
-    <t>0.2514460881761538</t>
-  </si>
-  <si>
     <t>E_of_T_L</t>
   </si>
   <si>
@@ -161,75 +131,21 @@
     <t>1.22+/-0.09</t>
   </si>
   <si>
-    <t>1.282+/-0.028</t>
-  </si>
-  <si>
-    <t>0.0074958389932654</t>
-  </si>
-  <si>
-    <t>-0.0023852565745502</t>
-  </si>
-  <si>
-    <t>0.0007635269888392</t>
-  </si>
-  <si>
     <t>E_of_L_T</t>
   </si>
   <si>
     <t>91</t>
   </si>
   <si>
-    <t>0.747+/-0.011</t>
-  </si>
-  <si>
-    <t>1.210+/-0.006</t>
-  </si>
-  <si>
-    <t>0.0001123488944888</t>
-  </si>
-  <si>
-    <t>6.416965439293787e-05</t>
-  </si>
-  <si>
-    <t>3.744555092302127e-05</t>
-  </si>
-  <si>
     <t>E_of_L_S</t>
   </si>
   <si>
-    <t>1.0+/-0.5</t>
-  </si>
-  <si>
-    <t>1.8+/-1.0</t>
-  </si>
-  <si>
-    <t>0.237227516911357</t>
-  </si>
-  <si>
-    <t>0.4442027637374247</t>
-  </si>
-  <si>
-    <t>1.0625428893165414</t>
-  </si>
-  <si>
     <t>E_of_S_L</t>
   </si>
   <si>
-    <t>0.70+/-0.08</t>
-  </si>
-  <si>
     <t>2.05+/-0.04</t>
   </si>
   <si>
-    <t>0.0058867513953671</t>
-  </si>
-  <si>
-    <t>-0.0032084265491169</t>
-  </si>
-  <si>
-    <t>0.0017654771478262</t>
-  </si>
-  <si>
     <t>P_of_T</t>
   </si>
   <si>
@@ -242,21 +158,6 @@
     <t>191</t>
   </si>
   <si>
-    <t>(9.74+/-0.35)e+03</t>
-  </si>
-  <si>
-    <t>2.175+/-0.010</t>
-  </si>
-  <si>
-    <t>124914.92862361252</t>
-  </si>
-  <si>
-    <t>3.406267361336492</t>
-  </si>
-  <si>
-    <t>9.363937944856796e-05</t>
-  </si>
-  <si>
     <t>P_of_L</t>
   </si>
   <si>
@@ -266,21 +167,6 @@
     <t>51</t>
   </si>
   <si>
-    <t>(9.2+/-0.6)e+03</t>
-  </si>
-  <si>
-    <t>2.130+/-0.019</t>
-  </si>
-  <si>
-    <t>315349.40624558576</t>
-  </si>
-  <si>
-    <t>10.66759804005478</t>
-  </si>
-  <si>
-    <t>0.0003615408963552</t>
-  </si>
-  <si>
     <t>P_of_S</t>
   </si>
   <si>
@@ -290,21 +176,6 @@
     <t>491</t>
   </si>
   <si>
-    <t>(6.16+/-0.15)e+03</t>
-  </si>
-  <si>
-    <t>2.140+/-0.005</t>
-  </si>
-  <si>
-    <t>22505.33441126952</t>
-  </si>
-  <si>
-    <t>0.811900407333634</t>
-  </si>
-  <si>
-    <t>2.9873877338451627e-05</t>
-  </si>
-  <si>
     <t>gamma 1</t>
   </si>
   <si>
@@ -324,6 +195,135 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>1.408+/-0.009</t>
+  </si>
+  <si>
+    <t>0.500+/-0.005</t>
+  </si>
+  <si>
+    <t>0.747+/-0.007</t>
+  </si>
+  <si>
+    <t>0.974+/-0.008</t>
+  </si>
+  <si>
+    <t>0.71+/-0.07</t>
+  </si>
+  <si>
+    <t>(9.74+/-0.30)e+03</t>
+  </si>
+  <si>
+    <t>(9.2+/-0.5)e+03</t>
+  </si>
+  <si>
+    <t>(6.16+/-0.26)e+03</t>
+  </si>
+  <si>
+    <t>1.538+/-0.004</t>
+  </si>
+  <si>
+    <t>8.245067465839669e-05</t>
+  </si>
+  <si>
+    <t>3.2295884083882994e-05</t>
+  </si>
+  <si>
+    <t>1.3762858929548115e-05</t>
+  </si>
+  <si>
+    <t>1.6005+/-0.0026</t>
+  </si>
+  <si>
+    <t>2.7862640835183355e-05</t>
+  </si>
+  <si>
+    <t>-1.3361267743955402e-05</t>
+  </si>
+  <si>
+    <t>6.833713372598827e-06</t>
+  </si>
+  <si>
+    <t>1.281+/-0.027</t>
+  </si>
+  <si>
+    <t>0.0077062871339481</t>
+  </si>
+  <si>
+    <t>-0.0023409044649269</t>
+  </si>
+  <si>
+    <t>0.0007152959738595</t>
+  </si>
+  <si>
+    <t>1.210+/-0.004</t>
+  </si>
+  <si>
+    <t>4.240773540447256e-05</t>
+  </si>
+  <si>
+    <t>2.41387603756598e-05</t>
+  </si>
+  <si>
+    <t>1.450686425197144e-05</t>
+  </si>
+  <si>
+    <t>1.845+/-0.007</t>
+  </si>
+  <si>
+    <t>5.959138836728755e-05</t>
+  </si>
+  <si>
+    <t>4.927804171350449e-05</t>
+  </si>
+  <si>
+    <t>4.264104846497495e-05</t>
+  </si>
+  <si>
+    <t>0.0045771396169808</t>
+  </si>
+  <si>
+    <t>-0.0024681255535876</t>
+  </si>
+  <si>
+    <t>0.0013463779974387</t>
+  </si>
+  <si>
+    <t>2.175+/-0.008</t>
+  </si>
+  <si>
+    <t>91878.36012172607</t>
+  </si>
+  <si>
+    <t>2.5100179083594862</t>
+  </si>
+  <si>
+    <t>6.920953669559218e-05</t>
+  </si>
+  <si>
+    <t>2.130+/-0.018</t>
+  </si>
+  <si>
+    <t>289617.5667288371</t>
+  </si>
+  <si>
+    <t>9.784496555159244</t>
+  </si>
+  <si>
+    <t>0.0003313867267222</t>
+  </si>
+  <si>
+    <t>2.140+/-0.010</t>
+  </si>
+  <si>
+    <t>68025.57078717892</t>
+  </si>
+  <si>
+    <t>2.54910351319638</t>
+  </si>
+  <si>
+    <t>9.72592645446996e-05</t>
   </si>
 </sst>
 </file>
@@ -760,7 +760,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +811,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -834,43 +834,43 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="K2" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="O2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -881,13 +881,13 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -902,22 +902,22 @@
         <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="K3" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="O3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -928,43 +928,43 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="O4" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -975,43 +975,43 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="L5" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="M5" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="N5" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="O5" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1022,43 +1022,43 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K6" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="M6" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="N6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="O6" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1069,43 +1069,43 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
         <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="L7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M7" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="N7" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="O7" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1116,43 +1116,43 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
         <v>22</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="L8" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="M8" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="N8" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="O8" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1163,43 +1163,43 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
         <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>63</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="I9" t="s">
         <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="L9" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="M9" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="N9" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="O9" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1210,43 +1210,43 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="I10" t="s">
         <v>22</v>
       </c>
       <c r="J10" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" t="s">
         <v>90</v>
       </c>
-      <c r="L10" t="s">
-        <v>83</v>
-      </c>
       <c r="M10" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="N10" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="O10" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>